<commit_message>
Commit 3: Final Drafts of Math and CS Visualizations in both BGWP and Color
Added Math Dep to dataset; Added Color to CS Visualization; Completed
Math Visualization
</commit_message>
<xml_diff>
--- a/Growth of MathCS Data.xlsx
+++ b/Growth of MathCS Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="6430"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="6430" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CS Related" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
   <si>
     <t>Math CS</t>
   </si>
@@ -94,6 +94,24 @@
   </si>
   <si>
     <t>Human-Computer Interaction (COGS)</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>Applied Math</t>
+  </si>
+  <si>
+    <t>Math/Econ</t>
+  </si>
+  <si>
+    <t>Secondary Education</t>
+  </si>
+  <si>
+    <t>Applied Sciences</t>
+  </si>
+  <si>
+    <t>Probability and Statistics</t>
   </si>
 </sst>
 </file>
@@ -413,7 +431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -817,129 +835,405 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="8.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2">
+        <v>73</v>
+      </c>
+      <c r="D2">
+        <v>39</v>
+      </c>
+      <c r="E2">
+        <v>166</v>
+      </c>
+      <c r="F2">
+        <v>117</v>
+      </c>
+      <c r="G2">
+        <v>21</v>
+      </c>
+      <c r="H2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3">
+        <v>80</v>
+      </c>
+      <c r="D3">
+        <v>36</v>
+      </c>
+      <c r="E3">
+        <v>152</v>
+      </c>
+      <c r="F3">
+        <v>118</v>
+      </c>
+      <c r="G3">
+        <v>17</v>
+      </c>
+      <c r="H3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <v>86</v>
+      </c>
+      <c r="D4">
+        <v>37</v>
+      </c>
+      <c r="E4">
+        <v>131</v>
+      </c>
+      <c r="F4">
+        <v>114</v>
+      </c>
+      <c r="G4">
+        <v>14</v>
+      </c>
+      <c r="H4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5">
+        <v>125</v>
+      </c>
+      <c r="D5">
+        <v>40</v>
+      </c>
+      <c r="E5">
+        <v>145</v>
+      </c>
+      <c r="F5">
+        <v>136</v>
+      </c>
+      <c r="G5">
+        <v>21</v>
+      </c>
+      <c r="H5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <v>135</v>
+      </c>
+      <c r="D6">
+        <v>36</v>
+      </c>
+      <c r="E6">
+        <v>124</v>
+      </c>
+      <c r="F6">
+        <v>147</v>
+      </c>
+      <c r="G6">
+        <v>18</v>
+      </c>
+      <c r="H6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7">
+        <v>136</v>
+      </c>
+      <c r="D7">
+        <v>35</v>
+      </c>
+      <c r="E7">
+        <v>110</v>
+      </c>
+      <c r="F7">
+        <v>145</v>
+      </c>
+      <c r="G7">
+        <v>17</v>
+      </c>
+      <c r="H7">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8">
         <v>70</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C8">
+        <v>185</v>
+      </c>
+      <c r="D8">
+        <v>35</v>
+      </c>
+      <c r="E8">
+        <v>149</v>
+      </c>
+      <c r="F8">
+        <v>167</v>
+      </c>
+      <c r="G8">
+        <v>31</v>
+      </c>
+      <c r="H8">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9">
         <v>84</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9">
+        <v>200</v>
+      </c>
+      <c r="D9">
+        <v>34</v>
+      </c>
+      <c r="E9">
+        <v>130</v>
+      </c>
+      <c r="F9">
+        <v>164</v>
+      </c>
+      <c r="G9">
+        <v>26</v>
+      </c>
+      <c r="H9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
         <v>91</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C10">
+        <v>189</v>
+      </c>
+      <c r="D10">
+        <v>37</v>
+      </c>
+      <c r="E10">
+        <v>121</v>
+      </c>
+      <c r="F10">
+        <v>163</v>
+      </c>
+      <c r="G10">
+        <v>24</v>
+      </c>
+      <c r="H10">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11">
         <v>193</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C11">
+        <v>299</v>
+      </c>
+      <c r="D11">
+        <v>42</v>
+      </c>
+      <c r="E11">
+        <v>182</v>
+      </c>
+      <c r="F11">
+        <v>156</v>
+      </c>
+      <c r="G11">
+        <v>44</v>
+      </c>
+      <c r="H11">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12">
         <v>246</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C12">
+        <v>313</v>
+      </c>
+      <c r="D12">
+        <v>36</v>
+      </c>
+      <c r="E12">
+        <v>155</v>
+      </c>
+      <c r="F12">
+        <v>158</v>
+      </c>
+      <c r="G12">
+        <v>45</v>
+      </c>
+      <c r="H12">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13">
         <v>293</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C13">
+        <v>311</v>
+      </c>
+      <c r="D13">
+        <v>31</v>
+      </c>
+      <c r="E13">
+        <v>147</v>
+      </c>
+      <c r="F13">
+        <v>170</v>
+      </c>
+      <c r="G13">
+        <v>31</v>
+      </c>
+      <c r="H13">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14">
         <v>602</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C14">
+        <v>417</v>
+      </c>
+      <c r="D14">
+        <v>40</v>
+      </c>
+      <c r="E14">
+        <v>219</v>
+      </c>
+      <c r="F14">
+        <v>192</v>
+      </c>
+      <c r="G14">
+        <v>46</v>
+      </c>
+      <c r="H14">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15">
         <v>747</v>
+      </c>
+      <c r="C15">
+        <v>409</v>
+      </c>
+      <c r="D15">
+        <v>37</v>
+      </c>
+      <c r="E15">
+        <v>211</v>
+      </c>
+      <c r="F15">
+        <v>241</v>
+      </c>
+      <c r="G15">
+        <v>46</v>
+      </c>
+      <c r="H15">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>